<commit_message>
Adding extra page factories
</commit_message>
<xml_diff>
--- a/Automation task_AFIT company/LinkedInUserData.xlsx
+++ b/Automation task_AFIT company/LinkedInUserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{24758B51-3A01-4A84-9528-7F3DC78ED5F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AAB7C38B-6703-45C1-BACE-1A42275A5F93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>First name</t>
   </si>
@@ -34,27 +34,15 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Islam</t>
-  </si>
-  <si>
-    <t>Abd Alazez</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
     <t>Ahmed</t>
   </si>
   <si>
-    <t>Hamed</t>
-  </si>
-  <si>
     <t>Ali</t>
   </si>
   <si>
-    <t>Yasser</t>
-  </si>
-  <si>
     <t>P@ssw0rd85</t>
   </si>
   <si>
@@ -73,13 +61,22 @@
     <t>Postal Code</t>
   </si>
   <si>
-    <t>afit19@gmail.com</t>
-  </si>
-  <si>
-    <t>afit29@gmail.com</t>
-  </si>
-  <si>
-    <t>afit39@gmail.com</t>
+    <t>Waleed</t>
+  </si>
+  <si>
+    <t>fadel</t>
+  </si>
+  <si>
+    <t>Gamal</t>
+  </si>
+  <si>
+    <t>ali89afit@gmail.com</t>
+  </si>
+  <si>
+    <t>gamal79afit@gmail.com</t>
+  </si>
+  <si>
+    <t>islamtalkha83@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -411,14 +408,14 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -438,27 +435,27 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>35681</v>
@@ -466,19 +463,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>35111</v>
@@ -486,19 +483,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>12018</v>

</xml_diff>

<commit_message>
Forget password almost done
</commit_message>
<xml_diff>
--- a/Automation task_AFIT company/LinkedInUserData.xlsx
+++ b/Automation task_AFIT company/LinkedInUserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{BA97FCAD-481B-4DB4-8E8F-62C0E4AD2BCC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AC74AC7D-44FF-4C55-8C98-F01CC2CDE951}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -409,7 +408,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +472,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Start merging page factories
</commit_message>
<xml_diff>
--- a/Automation task_AFIT company/LinkedInUserData.xlsx
+++ b/Automation task_AFIT company/LinkedInUserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AC74AC7D-44FF-4C55-8C98-F01CC2CDE951}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46526D4C-1540-4DF1-8314-8CE887F2E97E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>First name</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>P@ssw0rd</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
     <t>Ali</t>
   </si>
   <si>
@@ -67,23 +61,56 @@
     <t>fadel</t>
   </si>
   <si>
-    <t>Gamal</t>
-  </si>
-  <si>
     <t>ali89afit@gmail.com</t>
   </si>
   <si>
-    <t>gamal79afit@gmail.com</t>
-  </si>
-  <si>
     <t>islamtalkha83@gmail.com</t>
+  </si>
+  <si>
+    <t>Basem</t>
+  </si>
+  <si>
+    <t>basemhamdy1983@gmail.com</t>
+  </si>
+  <si>
+    <t>hamdy</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>QC Engineer</t>
+  </si>
+  <si>
+    <t>Arcom</t>
+  </si>
+  <si>
+    <t>Development Team Lead</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Work Industry</t>
+  </si>
+  <si>
+    <t>Information Technology and Services</t>
+  </si>
+  <si>
+    <t>Information Services</t>
+  </si>
+  <si>
+    <t>Hospital &amp; Health Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +125,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,9 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,23 +439,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,70 +472,106 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="F2">
         <v>35681</v>
       </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>35111</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>12018</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -507,9 +580,9 @@
     <hyperlink ref="D2" r:id="rId2" xr:uid="{796664A5-E543-4460-BB91-1FCFFBBB41EA}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{64F61F74-7062-4E14-9FB2-56E4BA2AEE1C}"/>
     <hyperlink ref="D3" r:id="rId4" xr:uid="{46437C6B-E4CB-4742-9445-B7BA1A7567FA}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{9470C683-C92F-4A83-BED0-F43BA45148DA}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{80AAAE69-2EB2-4D41-964C-AA49D9F43D74}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{80AAAE69-2EB2-4D41-964C-AA49D9F43D74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding get registration pin from mail subject functionality
</commit_message>
<xml_diff>
--- a/Automation task_AFIT company/LinkedInUserData.xlsx
+++ b/Automation task_AFIT company/LinkedInUserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46526D4C-1540-4DF1-8314-8CE887F2E97E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFEB0FC-64CD-4738-BC6E-FDFE5EE77184}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>First name</t>
   </si>
@@ -104,6 +104,39 @@
   </si>
   <si>
     <t>Hospital &amp; Health Care</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Elemam</t>
+  </si>
+  <si>
+    <t>aemamarcom83@gmail.com</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Alqemam</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Azez</t>
+  </si>
+  <si>
+    <t>islamazez83@gmail.com</t>
+  </si>
+  <si>
+    <t>Senior Software QC Engineer</t>
+  </si>
+  <si>
+    <t>ARCOM</t>
   </si>
 </sst>
 </file>
@@ -439,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +486,7 @@
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -571,6 +604,64 @@
         <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>155147</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>35111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -581,8 +672,12 @@
     <hyperlink ref="C3" r:id="rId3" xr:uid="{64F61F74-7062-4E14-9FB2-56E4BA2AEE1C}"/>
     <hyperlink ref="D3" r:id="rId4" xr:uid="{46437C6B-E4CB-4742-9445-B7BA1A7567FA}"/>
     <hyperlink ref="D4" r:id="rId5" xr:uid="{80AAAE69-2EB2-4D41-964C-AA49D9F43D74}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{9AF82C38-1EB6-4C3C-89FC-B66CC27C1193}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{633E8BE1-E7DD-4B3B-B260-BD8938C47B37}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{10EB7A7C-A2FC-4E54-A203-95D816C01783}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{EACE8712-584F-4D81-98FC-ADE0862E188C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding additional headers and add buttons to the profileEditPageFactory
</commit_message>
<xml_diff>
--- a/Automation task_AFIT company/LinkedInUserData.xlsx
+++ b/Automation task_AFIT company/LinkedInUserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{70B00C64-9331-4C2E-85D8-CE41E0E72AD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{689B0C25-3030-43B2-9DF7-F702E45FDDCE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>First name</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Hisham</t>
+  </si>
+  <si>
+    <t>Shahin</t>
+  </si>
+  <si>
+    <t>Nitco</t>
+  </si>
+  <si>
+    <t>hishamarcom1985@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -499,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,88 +677,117 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>151214</v>
+        <v>224455</v>
       </c>
       <c r="G6" t="s">
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F7">
-        <v>12345</v>
+        <v>151214</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F8">
-        <v>35111</v>
+        <v>12345</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>35111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -759,13 +800,15 @@
     <hyperlink ref="D4" r:id="rId5" xr:uid="{80AAAE69-2EB2-4D41-964C-AA49D9F43D74}"/>
     <hyperlink ref="C5" r:id="rId6" xr:uid="{9AF82C38-1EB6-4C3C-89FC-B66CC27C1193}"/>
     <hyperlink ref="D5" r:id="rId7" xr:uid="{633E8BE1-E7DD-4B3B-B260-BD8938C47B37}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{10EB7A7C-A2FC-4E54-A203-95D816C01783}"/>
-    <hyperlink ref="C8" r:id="rId9" xr:uid="{EACE8712-584F-4D81-98FC-ADE0862E188C}"/>
-    <hyperlink ref="D7" r:id="rId10" xr:uid="{EF588A81-E12F-4A51-B7DC-8735DD5DD953}"/>
-    <hyperlink ref="C6" r:id="rId11" xr:uid="{615E8D25-EC39-49A3-B7A4-A49782169F06}"/>
-    <hyperlink ref="D6" r:id="rId12" xr:uid="{06C22279-D403-4D46-A019-7905478A99D9}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{10EB7A7C-A2FC-4E54-A203-95D816C01783}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{EACE8712-584F-4D81-98FC-ADE0862E188C}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{EF588A81-E12F-4A51-B7DC-8735DD5DD953}"/>
+    <hyperlink ref="C7" r:id="rId11" xr:uid="{615E8D25-EC39-49A3-B7A4-A49782169F06}"/>
+    <hyperlink ref="D7" r:id="rId12" xr:uid="{06C22279-D403-4D46-A019-7905478A99D9}"/>
+    <hyperlink ref="C6" r:id="rId13" xr:uid="{BC1618FC-838B-44B7-B94B-D23C28A2C880}"/>
+    <hyperlink ref="D6" r:id="rId14" xr:uid="{8D7B077B-CC2B-49FB-919D-DD7F954159B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>